<commit_message>
update apis for getting all departments
</commit_message>
<xml_diff>
--- a/Department.xlsx
+++ b/Department.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RolesStructure\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7230"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14240" windowHeight="2020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>Role 1</t>
   </si>
@@ -69,22 +65,19 @@
     <t>Architect</t>
   </si>
   <si>
-    <t>Technical Lead</t>
-  </si>
-  <si>
-    <t>SW Delivery Manager</t>
-  </si>
-  <si>
-    <t>Team Lead</t>
-  </si>
-  <si>
-    <t>Product Manager</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>PS-EC</t>
+  </si>
+  <si>
+    <t>NE-EM</t>
+  </si>
+  <si>
+    <t>AS</t>
   </si>
 </sst>
 </file>
@@ -417,8 +410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -432,10 +425,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -443,7 +436,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -451,7 +444,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -459,24 +452,14 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
+      <c r="A5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
+      <c r="A6" s="1"/>
     </row>
     <row r="14" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="G14" s="3"/>

</xml_diff>

<commit_message>
added js file and update excel data
</commit_message>
<xml_diff>
--- a/Department.xlsx
+++ b/Department.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRA81HC\Desktop\test\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14240" windowHeight="2020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7230"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Role 1</t>
   </si>
@@ -78,6 +82,18 @@
   </si>
   <si>
     <t>AS</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>CC</t>
   </si>
 </sst>
 </file>
@@ -410,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -456,10 +472,36 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="G14" s="3"/>

</xml_diff>

<commit_message>
update back-end for structure
</commit_message>
<xml_diff>
--- a/Department.xlsx
+++ b/Department.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRA81HC\Desktop\test\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RolesStructure\project\orgchart\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,7 +13,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,47 +24,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
-  <si>
-    <t>Role 1</t>
-  </si>
-  <si>
-    <t>Role 2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
   <si>
     <t>Member Engineering</t>
   </si>
   <si>
-    <t>Technical Specialist</t>
-  </si>
-  <si>
-    <t>Delivery Lead</t>
-  </si>
-  <si>
-    <t>Lead Program Manager</t>
-  </si>
-  <si>
-    <t>Delivery Head</t>
-  </si>
-  <si>
     <t>Engineering Manager</t>
   </si>
   <si>
-    <t>Resource Manager</t>
-  </si>
-  <si>
     <t>DQA</t>
   </si>
   <si>
     <t>SQM</t>
   </si>
   <si>
-    <t>Lead Architect</t>
-  </si>
-  <si>
-    <t>Program manager</t>
-  </si>
-  <si>
     <t>Architect</t>
   </si>
   <si>
@@ -75,25 +47,82 @@
     <t>name</t>
   </si>
   <si>
-    <t>PS-EC</t>
-  </si>
-  <si>
-    <t>NE-EM</t>
-  </si>
-  <si>
-    <t>AS</t>
-  </si>
-  <si>
-    <t>Hardware</t>
-  </si>
-  <si>
-    <t>AE</t>
-  </si>
-  <si>
-    <t>CM</t>
-  </si>
-  <si>
-    <t>CC</t>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>ETM</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>ETI</t>
+  </si>
+  <si>
+    <t>ENG</t>
+  </si>
+  <si>
+    <t>EVH</t>
+  </si>
+  <si>
+    <t>EJV</t>
+  </si>
+  <si>
+    <t>ESS</t>
+  </si>
+  <si>
+    <t>EPS</t>
+  </si>
+  <si>
+    <t>Level 0</t>
+  </si>
+  <si>
+    <t>level 1</t>
+  </si>
+  <si>
+    <t>level 2</t>
+  </si>
+  <si>
+    <t>Level 3</t>
+  </si>
+  <si>
+    <t>Level 4</t>
+  </si>
+  <si>
+    <t>Level 5</t>
+  </si>
+  <si>
+    <t>Level 6</t>
+  </si>
+  <si>
+    <t>Level 7</t>
+  </si>
+  <si>
+    <t>Technical Lead</t>
+  </si>
+  <si>
+    <t>Product Manager</t>
+  </si>
+  <si>
+    <t>SW Delivery Manager</t>
+  </si>
+  <si>
+    <t>Team Lead</t>
+  </si>
+  <si>
+    <t>Subject Matter Expert</t>
+  </si>
+  <si>
+    <t>Principal Consultant</t>
+  </si>
+  <si>
+    <t>Program Manager</t>
+  </si>
+  <si>
+    <t>Principal Technologist</t>
   </si>
 </sst>
 </file>
@@ -135,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -144,6 +173,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,14 +454,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="16.90625" customWidth="1"/>
     <col min="4" max="4" width="25.08984375" customWidth="1"/>
     <col min="5" max="6" width="23.453125" customWidth="1"/>
@@ -439,80 +470,272 @@
     <col min="8" max="8" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="M3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4"/>
+      <c r="M4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="M5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="M6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="M7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" ht="13" x14ac:dyDescent="0.3">
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="M8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="I16" s="2"/>
+      <c r="D16" s="1"/>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
@@ -526,140 +749,28 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="25" spans="3:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="C25" s="3"/>
+    <row r="23" spans="3:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="C23" s="3"/>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="1"/>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C29" s="1"/>
-    </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:G3 D4:K8 E2:I2">
+      <formula1>$K$1:$K$13</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
+      <formula1>$M$1:$M$8</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:H8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>